<commit_message>
add axi_buzzer with api
</commit_message>
<xml_diff>
--- a/hw/buzzer/documentation/buzzer_addr_space.xlsx
+++ b/hw/buzzer/documentation/buzzer_addr_space.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\github\zturn\hw\buzzer\documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\github\zturn\hw\buzzer\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="15">
   <si>
     <t>Reg Number</t>
   </si>
@@ -66,12 +66,15 @@
   </si>
   <si>
     <t>MODE</t>
+  </si>
+  <si>
+    <t>BUZZER_ACTIVE</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -104,7 +107,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -153,11 +156,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -172,16 +186,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -196,11 +204,23 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -485,13 +505,13 @@
   <dimension ref="A1:AI12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="AL4" sqref="AL4"/>
+      <selection activeCell="C2" sqref="C2:Q2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.140625" style="1"/>
+    <col min="2" max="2" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="34" width="2.85546875" style="1" customWidth="1"/>
     <col min="35" max="35" width="6.85546875" style="1" bestFit="1" customWidth="1"/>
   </cols>
@@ -603,48 +623,52 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:35" ht="34.5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:35" ht="66.75" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
         <v>0</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="6"/>
-      <c r="E2" s="6"/>
-      <c r="F2" s="6"/>
-      <c r="G2" s="6"/>
-      <c r="H2" s="6"/>
-      <c r="I2" s="6"/>
-      <c r="J2" s="6"/>
-      <c r="K2" s="6"/>
-      <c r="L2" s="6"/>
-      <c r="M2" s="6"/>
-      <c r="N2" s="6"/>
-      <c r="O2" s="6"/>
-      <c r="P2" s="6"/>
-      <c r="Q2" s="6"/>
-      <c r="R2" s="6"/>
-      <c r="S2" s="6"/>
-      <c r="T2" s="6"/>
-      <c r="U2" s="6"/>
-      <c r="V2" s="6"/>
-      <c r="W2" s="6"/>
-      <c r="X2" s="6"/>
-      <c r="Y2" s="6"/>
-      <c r="Z2" s="6"/>
-      <c r="AA2" s="6"/>
-      <c r="AB2" s="6"/>
-      <c r="AC2" s="6"/>
-      <c r="AD2" s="6"/>
-      <c r="AE2" s="14" t="s">
+      <c r="D2" s="16"/>
+      <c r="E2" s="16"/>
+      <c r="F2" s="16"/>
+      <c r="G2" s="16"/>
+      <c r="H2" s="16"/>
+      <c r="I2" s="16"/>
+      <c r="J2" s="16"/>
+      <c r="K2" s="16"/>
+      <c r="L2" s="16"/>
+      <c r="M2" s="16"/>
+      <c r="N2" s="16"/>
+      <c r="O2" s="16"/>
+      <c r="P2" s="16"/>
+      <c r="Q2" s="17"/>
+      <c r="R2" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="S2" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="T2" s="16"/>
+      <c r="U2" s="16"/>
+      <c r="V2" s="16"/>
+      <c r="W2" s="16"/>
+      <c r="X2" s="16"/>
+      <c r="Y2" s="16"/>
+      <c r="Z2" s="16"/>
+      <c r="AA2" s="16"/>
+      <c r="AB2" s="16"/>
+      <c r="AC2" s="16"/>
+      <c r="AD2" s="17"/>
+      <c r="AE2" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="AF2" s="15"/>
-      <c r="AG2" s="9" t="s">
+      <c r="AF2" s="14"/>
+      <c r="AG2" s="7" t="s">
         <v>12</v>
       </c>
       <c r="AH2" s="5" t="s">
@@ -661,236 +685,236 @@
       <c r="B3" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="8" t="s">
+      <c r="C3" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="8"/>
-      <c r="E3" s="8"/>
-      <c r="F3" s="8"/>
-      <c r="G3" s="8"/>
-      <c r="H3" s="8"/>
-      <c r="I3" s="8"/>
-      <c r="J3" s="8"/>
-      <c r="K3" s="8"/>
-      <c r="L3" s="8"/>
-      <c r="M3" s="8"/>
-      <c r="N3" s="8"/>
-      <c r="O3" s="8"/>
-      <c r="P3" s="8"/>
-      <c r="Q3" s="8"/>
-      <c r="R3" s="8"/>
-      <c r="S3" s="8"/>
-      <c r="T3" s="8"/>
-      <c r="U3" s="8"/>
-      <c r="V3" s="8"/>
-      <c r="W3" s="8"/>
-      <c r="X3" s="8"/>
-      <c r="Y3" s="8"/>
-      <c r="Z3" s="8"/>
-      <c r="AA3" s="8"/>
-      <c r="AB3" s="8"/>
-      <c r="AC3" s="8"/>
-      <c r="AD3" s="8"/>
-      <c r="AE3" s="8"/>
-      <c r="AF3" s="8"/>
-      <c r="AG3" s="8"/>
-      <c r="AH3" s="8"/>
+      <c r="D3" s="12"/>
+      <c r="E3" s="12"/>
+      <c r="F3" s="12"/>
+      <c r="G3" s="12"/>
+      <c r="H3" s="12"/>
+      <c r="I3" s="12"/>
+      <c r="J3" s="12"/>
+      <c r="K3" s="12"/>
+      <c r="L3" s="12"/>
+      <c r="M3" s="12"/>
+      <c r="N3" s="12"/>
+      <c r="O3" s="12"/>
+      <c r="P3" s="12"/>
+      <c r="Q3" s="12"/>
+      <c r="R3" s="12"/>
+      <c r="S3" s="12"/>
+      <c r="T3" s="12"/>
+      <c r="U3" s="12"/>
+      <c r="V3" s="12"/>
+      <c r="W3" s="12"/>
+      <c r="X3" s="12"/>
+      <c r="Y3" s="12"/>
+      <c r="Z3" s="12"/>
+      <c r="AA3" s="12"/>
+      <c r="AB3" s="12"/>
+      <c r="AC3" s="12"/>
+      <c r="AD3" s="12"/>
+      <c r="AE3" s="12"/>
+      <c r="AF3" s="12"/>
+      <c r="AG3" s="12"/>
+      <c r="AH3" s="12"/>
       <c r="AI3" s="3" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A4" s="7">
+      <c r="A4" s="6">
         <v>2</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="B4" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="8" t="s">
+      <c r="C4" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="8"/>
-      <c r="E4" s="8"/>
-      <c r="F4" s="8"/>
-      <c r="G4" s="8"/>
-      <c r="H4" s="8"/>
-      <c r="I4" s="8"/>
-      <c r="J4" s="8"/>
-      <c r="K4" s="8"/>
-      <c r="L4" s="8"/>
-      <c r="M4" s="8"/>
-      <c r="N4" s="8"/>
-      <c r="O4" s="8"/>
-      <c r="P4" s="8"/>
-      <c r="Q4" s="8"/>
-      <c r="R4" s="8"/>
-      <c r="S4" s="8"/>
-      <c r="T4" s="8"/>
-      <c r="U4" s="8"/>
-      <c r="V4" s="8"/>
-      <c r="W4" s="8"/>
-      <c r="X4" s="8"/>
-      <c r="Y4" s="8"/>
-      <c r="Z4" s="8"/>
-      <c r="AA4" s="8"/>
-      <c r="AB4" s="8"/>
-      <c r="AC4" s="8"/>
-      <c r="AD4" s="8"/>
-      <c r="AE4" s="8"/>
-      <c r="AF4" s="8"/>
-      <c r="AG4" s="8"/>
-      <c r="AH4" s="8"/>
-      <c r="AI4" s="7" t="s">
+      <c r="D4" s="12"/>
+      <c r="E4" s="12"/>
+      <c r="F4" s="12"/>
+      <c r="G4" s="12"/>
+      <c r="H4" s="12"/>
+      <c r="I4" s="12"/>
+      <c r="J4" s="12"/>
+      <c r="K4" s="12"/>
+      <c r="L4" s="12"/>
+      <c r="M4" s="12"/>
+      <c r="N4" s="12"/>
+      <c r="O4" s="12"/>
+      <c r="P4" s="12"/>
+      <c r="Q4" s="12"/>
+      <c r="R4" s="12"/>
+      <c r="S4" s="12"/>
+      <c r="T4" s="12"/>
+      <c r="U4" s="12"/>
+      <c r="V4" s="12"/>
+      <c r="W4" s="12"/>
+      <c r="X4" s="12"/>
+      <c r="Y4" s="12"/>
+      <c r="Z4" s="12"/>
+      <c r="AA4" s="12"/>
+      <c r="AB4" s="12"/>
+      <c r="AC4" s="12"/>
+      <c r="AD4" s="12"/>
+      <c r="AE4" s="12"/>
+      <c r="AF4" s="12"/>
+      <c r="AG4" s="12"/>
+      <c r="AH4" s="12"/>
+      <c r="AI4" s="6" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A5" s="10"/>
-      <c r="B5" s="10"/>
-      <c r="C5" s="11"/>
-      <c r="D5" s="11"/>
-      <c r="E5" s="11"/>
-      <c r="F5" s="11"/>
-      <c r="G5" s="11"/>
-      <c r="H5" s="11"/>
-      <c r="I5" s="11"/>
-      <c r="J5" s="11"/>
-      <c r="K5" s="11"/>
-      <c r="L5" s="11"/>
-      <c r="M5" s="11"/>
-      <c r="N5" s="11"/>
-      <c r="O5" s="11"/>
-      <c r="P5" s="11"/>
-      <c r="Q5" s="11"/>
-      <c r="R5" s="11"/>
-      <c r="S5" s="11"/>
-      <c r="T5" s="11"/>
-      <c r="U5" s="11"/>
-      <c r="V5" s="11"/>
-      <c r="W5" s="11"/>
-      <c r="X5" s="11"/>
-      <c r="Y5" s="11"/>
-      <c r="Z5" s="11"/>
-      <c r="AA5" s="11"/>
-      <c r="AB5" s="11"/>
-      <c r="AC5" s="11"/>
-      <c r="AD5" s="11"/>
-      <c r="AE5" s="11"/>
-      <c r="AF5" s="12"/>
-      <c r="AG5" s="13"/>
-      <c r="AH5" s="13"/>
-      <c r="AI5" s="10"/>
+      <c r="A5" s="8"/>
+      <c r="B5" s="8"/>
+      <c r="C5" s="9"/>
+      <c r="D5" s="9"/>
+      <c r="E5" s="9"/>
+      <c r="F5" s="9"/>
+      <c r="G5" s="9"/>
+      <c r="H5" s="9"/>
+      <c r="I5" s="9"/>
+      <c r="J5" s="9"/>
+      <c r="K5" s="9"/>
+      <c r="L5" s="9"/>
+      <c r="M5" s="9"/>
+      <c r="N5" s="9"/>
+      <c r="O5" s="9"/>
+      <c r="P5" s="9"/>
+      <c r="Q5" s="9"/>
+      <c r="R5" s="9"/>
+      <c r="S5" s="9"/>
+      <c r="T5" s="9"/>
+      <c r="U5" s="9"/>
+      <c r="V5" s="9"/>
+      <c r="W5" s="9"/>
+      <c r="X5" s="9"/>
+      <c r="Y5" s="9"/>
+      <c r="Z5" s="9"/>
+      <c r="AA5" s="9"/>
+      <c r="AB5" s="9"/>
+      <c r="AC5" s="9"/>
+      <c r="AD5" s="9"/>
+      <c r="AE5" s="9"/>
+      <c r="AF5" s="10"/>
+      <c r="AG5" s="11"/>
+      <c r="AH5" s="11"/>
+      <c r="AI5" s="8"/>
     </row>
     <row r="6" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A6" s="10"/>
-      <c r="B6" s="10"/>
-      <c r="C6" s="11"/>
-      <c r="D6" s="11"/>
-      <c r="E6" s="11"/>
-      <c r="F6" s="11"/>
-      <c r="G6" s="11"/>
-      <c r="H6" s="11"/>
-      <c r="I6" s="11"/>
-      <c r="J6" s="11"/>
-      <c r="K6" s="11"/>
-      <c r="L6" s="11"/>
-      <c r="M6" s="11"/>
-      <c r="N6" s="11"/>
-      <c r="O6" s="11"/>
-      <c r="P6" s="11"/>
-      <c r="Q6" s="11"/>
-      <c r="R6" s="11"/>
-      <c r="S6" s="11"/>
-      <c r="T6" s="11"/>
-      <c r="U6" s="11"/>
-      <c r="V6" s="11"/>
-      <c r="W6" s="11"/>
-      <c r="X6" s="11"/>
-      <c r="Y6" s="11"/>
-      <c r="Z6" s="11"/>
-      <c r="AA6" s="11"/>
-      <c r="AB6" s="11"/>
-      <c r="AC6" s="11"/>
-      <c r="AD6" s="11"/>
-      <c r="AE6" s="11"/>
-      <c r="AF6" s="11"/>
-      <c r="AG6" s="11"/>
-      <c r="AH6" s="11"/>
-      <c r="AI6" s="10"/>
+      <c r="A6" s="8"/>
+      <c r="B6" s="8"/>
+      <c r="C6" s="9"/>
+      <c r="D6" s="9"/>
+      <c r="E6" s="9"/>
+      <c r="F6" s="9"/>
+      <c r="G6" s="9"/>
+      <c r="H6" s="9"/>
+      <c r="I6" s="9"/>
+      <c r="J6" s="9"/>
+      <c r="K6" s="9"/>
+      <c r="L6" s="9"/>
+      <c r="M6" s="9"/>
+      <c r="N6" s="9"/>
+      <c r="O6" s="9"/>
+      <c r="P6" s="9"/>
+      <c r="Q6" s="9"/>
+      <c r="R6" s="9"/>
+      <c r="S6" s="9"/>
+      <c r="T6" s="9"/>
+      <c r="U6" s="9"/>
+      <c r="V6" s="9"/>
+      <c r="W6" s="9"/>
+      <c r="X6" s="9"/>
+      <c r="Y6" s="9"/>
+      <c r="Z6" s="9"/>
+      <c r="AA6" s="9"/>
+      <c r="AB6" s="9"/>
+      <c r="AC6" s="9"/>
+      <c r="AD6" s="9"/>
+      <c r="AE6" s="9"/>
+      <c r="AF6" s="9"/>
+      <c r="AG6" s="9"/>
+      <c r="AH6" s="9"/>
+      <c r="AI6" s="8"/>
     </row>
     <row r="7" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A7" s="10"/>
-      <c r="B7" s="10"/>
-      <c r="C7" s="11"/>
-      <c r="D7" s="11"/>
-      <c r="E7" s="11"/>
-      <c r="F7" s="11"/>
-      <c r="G7" s="11"/>
-      <c r="H7" s="11"/>
-      <c r="I7" s="11"/>
-      <c r="J7" s="11"/>
-      <c r="K7" s="11"/>
-      <c r="L7" s="11"/>
-      <c r="M7" s="11"/>
-      <c r="N7" s="11"/>
-      <c r="O7" s="11"/>
-      <c r="P7" s="11"/>
-      <c r="Q7" s="11"/>
-      <c r="R7" s="11"/>
-      <c r="S7" s="11"/>
-      <c r="T7" s="11"/>
-      <c r="U7" s="11"/>
-      <c r="V7" s="11"/>
-      <c r="W7" s="11"/>
-      <c r="X7" s="11"/>
-      <c r="Y7" s="11"/>
-      <c r="Z7" s="11"/>
-      <c r="AA7" s="11"/>
-      <c r="AB7" s="11"/>
-      <c r="AC7" s="11"/>
-      <c r="AD7" s="11"/>
-      <c r="AE7" s="11"/>
-      <c r="AF7" s="12"/>
-      <c r="AG7" s="13"/>
-      <c r="AH7" s="13"/>
-      <c r="AI7" s="10"/>
+      <c r="A7" s="8"/>
+      <c r="B7" s="8"/>
+      <c r="C7" s="9"/>
+      <c r="D7" s="9"/>
+      <c r="E7" s="9"/>
+      <c r="F7" s="9"/>
+      <c r="G7" s="9"/>
+      <c r="H7" s="9"/>
+      <c r="I7" s="9"/>
+      <c r="J7" s="9"/>
+      <c r="K7" s="9"/>
+      <c r="L7" s="9"/>
+      <c r="M7" s="9"/>
+      <c r="N7" s="9"/>
+      <c r="O7" s="9"/>
+      <c r="P7" s="9"/>
+      <c r="Q7" s="9"/>
+      <c r="R7" s="9"/>
+      <c r="S7" s="9"/>
+      <c r="T7" s="9"/>
+      <c r="U7" s="9"/>
+      <c r="V7" s="9"/>
+      <c r="W7" s="9"/>
+      <c r="X7" s="9"/>
+      <c r="Y7" s="9"/>
+      <c r="Z7" s="9"/>
+      <c r="AA7" s="9"/>
+      <c r="AB7" s="9"/>
+      <c r="AC7" s="9"/>
+      <c r="AD7" s="9"/>
+      <c r="AE7" s="9"/>
+      <c r="AF7" s="10"/>
+      <c r="AG7" s="11"/>
+      <c r="AH7" s="11"/>
+      <c r="AI7" s="8"/>
     </row>
     <row r="8" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A8" s="10"/>
-      <c r="B8" s="10"/>
-      <c r="C8" s="11"/>
-      <c r="D8" s="11"/>
-      <c r="E8" s="11"/>
-      <c r="F8" s="11"/>
-      <c r="G8" s="11"/>
-      <c r="H8" s="11"/>
-      <c r="I8" s="11"/>
-      <c r="J8" s="11"/>
-      <c r="K8" s="11"/>
-      <c r="L8" s="11"/>
-      <c r="M8" s="11"/>
-      <c r="N8" s="11"/>
-      <c r="O8" s="11"/>
-      <c r="P8" s="11"/>
-      <c r="Q8" s="11"/>
-      <c r="R8" s="11"/>
-      <c r="S8" s="11"/>
-      <c r="T8" s="11"/>
-      <c r="U8" s="11"/>
-      <c r="V8" s="11"/>
-      <c r="W8" s="11"/>
-      <c r="X8" s="11"/>
-      <c r="Y8" s="11"/>
-      <c r="Z8" s="11"/>
-      <c r="AA8" s="11"/>
-      <c r="AB8" s="11"/>
-      <c r="AC8" s="11"/>
-      <c r="AD8" s="11"/>
-      <c r="AE8" s="11"/>
-      <c r="AF8" s="11"/>
-      <c r="AG8" s="11"/>
-      <c r="AH8" s="11"/>
-      <c r="AI8" s="10"/>
+      <c r="A8" s="8"/>
+      <c r="B8" s="8"/>
+      <c r="C8" s="9"/>
+      <c r="D8" s="9"/>
+      <c r="E8" s="9"/>
+      <c r="F8" s="9"/>
+      <c r="G8" s="9"/>
+      <c r="H8" s="9"/>
+      <c r="I8" s="9"/>
+      <c r="J8" s="9"/>
+      <c r="K8" s="9"/>
+      <c r="L8" s="9"/>
+      <c r="M8" s="9"/>
+      <c r="N8" s="9"/>
+      <c r="O8" s="9"/>
+      <c r="P8" s="9"/>
+      <c r="Q8" s="9"/>
+      <c r="R8" s="9"/>
+      <c r="S8" s="9"/>
+      <c r="T8" s="9"/>
+      <c r="U8" s="9"/>
+      <c r="V8" s="9"/>
+      <c r="W8" s="9"/>
+      <c r="X8" s="9"/>
+      <c r="Y8" s="9"/>
+      <c r="Z8" s="9"/>
+      <c r="AA8" s="9"/>
+      <c r="AB8" s="9"/>
+      <c r="AC8" s="9"/>
+      <c r="AD8" s="9"/>
+      <c r="AE8" s="9"/>
+      <c r="AF8" s="9"/>
+      <c r="AG8" s="9"/>
+      <c r="AH8" s="9"/>
+      <c r="AI8" s="8"/>
     </row>
     <row r="9" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A9" s="2"/>
@@ -1040,11 +1064,12 @@
       <c r="AH12" s="2"/>
     </row>
   </sheetData>
-  <mergeCells count="4">
-    <mergeCell ref="C2:AD2"/>
+  <mergeCells count="5">
     <mergeCell ref="C4:AH4"/>
     <mergeCell ref="C3:AH3"/>
     <mergeCell ref="AE2:AF2"/>
+    <mergeCell ref="C2:Q2"/>
+    <mergeCell ref="S2:AD2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>

</xml_diff>